<commit_message>
Created functions to get season record
I realized that my old code did not download the season record, just the team statistics!

I also created the functions to update the tables of each XLSX with their respective record.
</commit_message>
<xml_diff>
--- a/data/ARI_1998.xlsx
+++ b/data/ARI_1998.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AC48"/>
+  <dimension ref="A1:AF48"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -579,6 +579,21 @@
           <t>Unnamed: 28</t>
         </is>
       </c>
+      <c r="AD1" s="1" t="inlineStr">
+        <is>
+          <t>Wins</t>
+        </is>
+      </c>
+      <c r="AE1" s="1" t="inlineStr">
+        <is>
+          <t>Losses</t>
+        </is>
+      </c>
+      <c r="AF1" s="1" t="inlineStr">
+        <is>
+          <t>Ties</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -722,6 +737,15 @@
         </is>
       </c>
       <c r="AC2" t="inlineStr"/>
+      <c r="AD2" t="n">
+        <v>65</v>
+      </c>
+      <c r="AE2" t="n">
+        <v>97</v>
+      </c>
+      <c r="AF2" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -865,6 +889,15 @@
         </is>
       </c>
       <c r="AC3" t="inlineStr"/>
+      <c r="AD3" t="n">
+        <v>65</v>
+      </c>
+      <c r="AE3" t="n">
+        <v>97</v>
+      </c>
+      <c r="AF3" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -1004,6 +1037,15 @@
       </c>
       <c r="AB4" t="inlineStr"/>
       <c r="AC4" t="inlineStr"/>
+      <c r="AD4" t="n">
+        <v>65</v>
+      </c>
+      <c r="AE4" t="n">
+        <v>97</v>
+      </c>
+      <c r="AF4" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -1147,6 +1189,15 @@
         </is>
       </c>
       <c r="AC5" t="inlineStr"/>
+      <c r="AD5" t="n">
+        <v>65</v>
+      </c>
+      <c r="AE5" t="n">
+        <v>97</v>
+      </c>
+      <c r="AF5" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -1290,6 +1341,15 @@
         </is>
       </c>
       <c r="AC6" t="inlineStr"/>
+      <c r="AD6" t="n">
+        <v>65</v>
+      </c>
+      <c r="AE6" t="n">
+        <v>97</v>
+      </c>
+      <c r="AF6" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -1433,6 +1493,15 @@
         </is>
       </c>
       <c r="AC7" t="inlineStr"/>
+      <c r="AD7" t="n">
+        <v>65</v>
+      </c>
+      <c r="AE7" t="n">
+        <v>97</v>
+      </c>
+      <c r="AF7" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -1576,6 +1645,15 @@
         </is>
       </c>
       <c r="AC8" t="inlineStr"/>
+      <c r="AD8" t="n">
+        <v>65</v>
+      </c>
+      <c r="AE8" t="n">
+        <v>97</v>
+      </c>
+      <c r="AF8" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -1719,6 +1797,15 @@
         </is>
       </c>
       <c r="AC9" t="inlineStr"/>
+      <c r="AD9" t="n">
+        <v>65</v>
+      </c>
+      <c r="AE9" t="n">
+        <v>97</v>
+      </c>
+      <c r="AF9" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -1862,6 +1949,15 @@
         </is>
       </c>
       <c r="AC10" t="inlineStr"/>
+      <c r="AD10" t="n">
+        <v>65</v>
+      </c>
+      <c r="AE10" t="n">
+        <v>97</v>
+      </c>
+      <c r="AF10" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -2005,6 +2101,15 @@
         </is>
       </c>
       <c r="AC11" t="inlineStr"/>
+      <c r="AD11" t="n">
+        <v>65</v>
+      </c>
+      <c r="AE11" t="n">
+        <v>97</v>
+      </c>
+      <c r="AF11" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -2148,6 +2253,15 @@
         </is>
       </c>
       <c r="AC12" t="inlineStr"/>
+      <c r="AD12" t="n">
+        <v>65</v>
+      </c>
+      <c r="AE12" t="n">
+        <v>97</v>
+      </c>
+      <c r="AF12" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -2287,6 +2401,15 @@
       </c>
       <c r="AB13" t="inlineStr"/>
       <c r="AC13" t="inlineStr"/>
+      <c r="AD13" t="n">
+        <v>65</v>
+      </c>
+      <c r="AE13" t="n">
+        <v>97</v>
+      </c>
+      <c r="AF13" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -2430,6 +2553,15 @@
         </is>
       </c>
       <c r="AC14" t="inlineStr"/>
+      <c r="AD14" t="n">
+        <v>65</v>
+      </c>
+      <c r="AE14" t="n">
+        <v>97</v>
+      </c>
+      <c r="AF14" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -2573,6 +2705,15 @@
         </is>
       </c>
       <c r="AC15" t="inlineStr"/>
+      <c r="AD15" t="n">
+        <v>65</v>
+      </c>
+      <c r="AE15" t="n">
+        <v>97</v>
+      </c>
+      <c r="AF15" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -2716,6 +2857,15 @@
         </is>
       </c>
       <c r="AC16" t="inlineStr"/>
+      <c r="AD16" t="n">
+        <v>65</v>
+      </c>
+      <c r="AE16" t="n">
+        <v>97</v>
+      </c>
+      <c r="AF16" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -2855,6 +3005,15 @@
       </c>
       <c r="AB17" t="inlineStr"/>
       <c r="AC17" t="inlineStr"/>
+      <c r="AD17" t="n">
+        <v>65</v>
+      </c>
+      <c r="AE17" t="n">
+        <v>97</v>
+      </c>
+      <c r="AF17" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -2998,6 +3157,15 @@
         </is>
       </c>
       <c r="AC18" t="inlineStr"/>
+      <c r="AD18" t="n">
+        <v>65</v>
+      </c>
+      <c r="AE18" t="n">
+        <v>97</v>
+      </c>
+      <c r="AF18" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -3141,6 +3309,15 @@
         </is>
       </c>
       <c r="AC19" t="inlineStr"/>
+      <c r="AD19" t="n">
+        <v>65</v>
+      </c>
+      <c r="AE19" t="n">
+        <v>97</v>
+      </c>
+      <c r="AF19" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -3284,6 +3461,15 @@
         </is>
       </c>
       <c r="AC20" t="inlineStr"/>
+      <c r="AD20" t="n">
+        <v>65</v>
+      </c>
+      <c r="AE20" t="n">
+        <v>97</v>
+      </c>
+      <c r="AF20" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -3427,6 +3613,15 @@
         </is>
       </c>
       <c r="AC21" t="inlineStr"/>
+      <c r="AD21" t="n">
+        <v>65</v>
+      </c>
+      <c r="AE21" t="n">
+        <v>97</v>
+      </c>
+      <c r="AF21" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -3570,6 +3765,15 @@
         </is>
       </c>
       <c r="AC22" t="inlineStr"/>
+      <c r="AD22" t="n">
+        <v>65</v>
+      </c>
+      <c r="AE22" t="n">
+        <v>97</v>
+      </c>
+      <c r="AF22" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -3709,6 +3913,15 @@
       </c>
       <c r="AB23" t="inlineStr"/>
       <c r="AC23" t="inlineStr"/>
+      <c r="AD23" t="n">
+        <v>65</v>
+      </c>
+      <c r="AE23" t="n">
+        <v>97</v>
+      </c>
+      <c r="AF23" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -3852,6 +4065,15 @@
         </is>
       </c>
       <c r="AC24" t="inlineStr"/>
+      <c r="AD24" t="n">
+        <v>65</v>
+      </c>
+      <c r="AE24" t="n">
+        <v>97</v>
+      </c>
+      <c r="AF24" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -3991,6 +4213,15 @@
       </c>
       <c r="AB25" t="inlineStr"/>
       <c r="AC25" t="inlineStr"/>
+      <c r="AD25" t="n">
+        <v>65</v>
+      </c>
+      <c r="AE25" t="n">
+        <v>97</v>
+      </c>
+      <c r="AF25" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -4134,6 +4365,15 @@
         </is>
       </c>
       <c r="AC26" t="inlineStr"/>
+      <c r="AD26" t="n">
+        <v>65</v>
+      </c>
+      <c r="AE26" t="n">
+        <v>97</v>
+      </c>
+      <c r="AF26" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -4277,6 +4517,15 @@
         </is>
       </c>
       <c r="AC27" t="inlineStr"/>
+      <c r="AD27" t="n">
+        <v>65</v>
+      </c>
+      <c r="AE27" t="n">
+        <v>97</v>
+      </c>
+      <c r="AF27" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -4416,6 +4665,15 @@
       </c>
       <c r="AB28" t="inlineStr"/>
       <c r="AC28" t="inlineStr"/>
+      <c r="AD28" t="n">
+        <v>65</v>
+      </c>
+      <c r="AE28" t="n">
+        <v>97</v>
+      </c>
+      <c r="AF28" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -4559,6 +4817,15 @@
         </is>
       </c>
       <c r="AC29" t="inlineStr"/>
+      <c r="AD29" t="n">
+        <v>65</v>
+      </c>
+      <c r="AE29" t="n">
+        <v>97</v>
+      </c>
+      <c r="AF29" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -4702,6 +4969,15 @@
         </is>
       </c>
       <c r="AC30" t="inlineStr"/>
+      <c r="AD30" t="n">
+        <v>65</v>
+      </c>
+      <c r="AE30" t="n">
+        <v>97</v>
+      </c>
+      <c r="AF30" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -4841,6 +5117,15 @@
       </c>
       <c r="AB31" t="inlineStr"/>
       <c r="AC31" t="inlineStr"/>
+      <c r="AD31" t="n">
+        <v>65</v>
+      </c>
+      <c r="AE31" t="n">
+        <v>97</v>
+      </c>
+      <c r="AF31" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -4984,6 +5269,15 @@
         </is>
       </c>
       <c r="AC32" t="inlineStr"/>
+      <c r="AD32" t="n">
+        <v>65</v>
+      </c>
+      <c r="AE32" t="n">
+        <v>97</v>
+      </c>
+      <c r="AF32" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -5123,6 +5417,15 @@
       </c>
       <c r="AB33" t="inlineStr"/>
       <c r="AC33" t="inlineStr"/>
+      <c r="AD33" t="n">
+        <v>65</v>
+      </c>
+      <c r="AE33" t="n">
+        <v>97</v>
+      </c>
+      <c r="AF33" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -5262,6 +5565,15 @@
       </c>
       <c r="AB34" t="inlineStr"/>
       <c r="AC34" t="inlineStr"/>
+      <c r="AD34" t="n">
+        <v>65</v>
+      </c>
+      <c r="AE34" t="n">
+        <v>97</v>
+      </c>
+      <c r="AF34" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -5405,6 +5717,15 @@
         </is>
       </c>
       <c r="AC35" t="inlineStr"/>
+      <c r="AD35" t="n">
+        <v>65</v>
+      </c>
+      <c r="AE35" t="n">
+        <v>97</v>
+      </c>
+      <c r="AF35" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -5548,6 +5869,15 @@
         </is>
       </c>
       <c r="AC36" t="inlineStr"/>
+      <c r="AD36" t="n">
+        <v>65</v>
+      </c>
+      <c r="AE36" t="n">
+        <v>97</v>
+      </c>
+      <c r="AF36" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -5691,6 +6021,15 @@
         </is>
       </c>
       <c r="AC37" t="inlineStr"/>
+      <c r="AD37" t="n">
+        <v>65</v>
+      </c>
+      <c r="AE37" t="n">
+        <v>97</v>
+      </c>
+      <c r="AF37" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -5834,6 +6173,15 @@
         </is>
       </c>
       <c r="AC38" t="inlineStr"/>
+      <c r="AD38" t="n">
+        <v>65</v>
+      </c>
+      <c r="AE38" t="n">
+        <v>97</v>
+      </c>
+      <c r="AF38" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -5977,6 +6325,15 @@
         </is>
       </c>
       <c r="AC39" t="inlineStr"/>
+      <c r="AD39" t="n">
+        <v>65</v>
+      </c>
+      <c r="AE39" t="n">
+        <v>97</v>
+      </c>
+      <c r="AF39" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -6120,6 +6477,15 @@
         </is>
       </c>
       <c r="AC40" t="inlineStr"/>
+      <c r="AD40" t="n">
+        <v>65</v>
+      </c>
+      <c r="AE40" t="n">
+        <v>97</v>
+      </c>
+      <c r="AF40" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -6263,6 +6629,15 @@
         </is>
       </c>
       <c r="AC41" t="inlineStr"/>
+      <c r="AD41" t="n">
+        <v>65</v>
+      </c>
+      <c r="AE41" t="n">
+        <v>97</v>
+      </c>
+      <c r="AF41" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -6406,6 +6781,15 @@
         </is>
       </c>
       <c r="AC42" t="inlineStr"/>
+      <c r="AD42" t="n">
+        <v>65</v>
+      </c>
+      <c r="AE42" t="n">
+        <v>97</v>
+      </c>
+      <c r="AF42" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
@@ -6545,6 +6929,15 @@
       </c>
       <c r="AB43" t="inlineStr"/>
       <c r="AC43" t="inlineStr"/>
+      <c r="AD43" t="n">
+        <v>65</v>
+      </c>
+      <c r="AE43" t="n">
+        <v>97</v>
+      </c>
+      <c r="AF43" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
@@ -6684,6 +7077,15 @@
       </c>
       <c r="AB44" t="inlineStr"/>
       <c r="AC44" t="inlineStr"/>
+      <c r="AD44" t="n">
+        <v>65</v>
+      </c>
+      <c r="AE44" t="n">
+        <v>97</v>
+      </c>
+      <c r="AF44" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
@@ -6831,6 +7233,15 @@
           <t>All-Star</t>
         </is>
       </c>
+      <c r="AD45" t="n">
+        <v>65</v>
+      </c>
+      <c r="AE45" t="n">
+        <v>97</v>
+      </c>
+      <c r="AF45" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
@@ -6974,6 +7385,15 @@
         </is>
       </c>
       <c r="AC46" t="inlineStr"/>
+      <c r="AD46" t="n">
+        <v>65</v>
+      </c>
+      <c r="AE46" t="n">
+        <v>97</v>
+      </c>
+      <c r="AF46" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
@@ -7113,6 +7533,15 @@
       </c>
       <c r="AB47" t="inlineStr"/>
       <c r="AC47" t="inlineStr"/>
+      <c r="AD47" t="n">
+        <v>65</v>
+      </c>
+      <c r="AE47" t="n">
+        <v>97</v>
+      </c>
+      <c r="AF47" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
@@ -7252,6 +7681,15 @@
         </is>
       </c>
       <c r="AC48" t="inlineStr"/>
+      <c r="AD48" t="n">
+        <v>65</v>
+      </c>
+      <c r="AE48" t="n">
+        <v>97</v>
+      </c>
+      <c r="AF48" t="n">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Added team record to data
The data is a little different than website_scraper because the W/L/T are on the same sheet instead of a different sheet.
</commit_message>
<xml_diff>
--- a/data/ARI_1998.xlsx
+++ b/data/ARI_1998.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AC48"/>
+  <dimension ref="A1:AF48"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -579,6 +579,21 @@
           <t>Unnamed: 28</t>
         </is>
       </c>
+      <c r="AD1" s="1" t="inlineStr">
+        <is>
+          <t>Wins</t>
+        </is>
+      </c>
+      <c r="AE1" s="1" t="inlineStr">
+        <is>
+          <t>Losses</t>
+        </is>
+      </c>
+      <c r="AF1" s="1" t="inlineStr">
+        <is>
+          <t>Ties</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -722,6 +737,15 @@
         </is>
       </c>
       <c r="AC2" t="inlineStr"/>
+      <c r="AD2" t="n">
+        <v>65</v>
+      </c>
+      <c r="AE2" t="n">
+        <v>97</v>
+      </c>
+      <c r="AF2" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -865,6 +889,15 @@
         </is>
       </c>
       <c r="AC3" t="inlineStr"/>
+      <c r="AD3" t="n">
+        <v>65</v>
+      </c>
+      <c r="AE3" t="n">
+        <v>97</v>
+      </c>
+      <c r="AF3" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -1004,6 +1037,15 @@
       </c>
       <c r="AB4" t="inlineStr"/>
       <c r="AC4" t="inlineStr"/>
+      <c r="AD4" t="n">
+        <v>65</v>
+      </c>
+      <c r="AE4" t="n">
+        <v>97</v>
+      </c>
+      <c r="AF4" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -1147,6 +1189,15 @@
         </is>
       </c>
       <c r="AC5" t="inlineStr"/>
+      <c r="AD5" t="n">
+        <v>65</v>
+      </c>
+      <c r="AE5" t="n">
+        <v>97</v>
+      </c>
+      <c r="AF5" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -1290,6 +1341,15 @@
         </is>
       </c>
       <c r="AC6" t="inlineStr"/>
+      <c r="AD6" t="n">
+        <v>65</v>
+      </c>
+      <c r="AE6" t="n">
+        <v>97</v>
+      </c>
+      <c r="AF6" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -1433,6 +1493,15 @@
         </is>
       </c>
       <c r="AC7" t="inlineStr"/>
+      <c r="AD7" t="n">
+        <v>65</v>
+      </c>
+      <c r="AE7" t="n">
+        <v>97</v>
+      </c>
+      <c r="AF7" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -1576,6 +1645,15 @@
         </is>
       </c>
       <c r="AC8" t="inlineStr"/>
+      <c r="AD8" t="n">
+        <v>65</v>
+      </c>
+      <c r="AE8" t="n">
+        <v>97</v>
+      </c>
+      <c r="AF8" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -1719,6 +1797,15 @@
         </is>
       </c>
       <c r="AC9" t="inlineStr"/>
+      <c r="AD9" t="n">
+        <v>65</v>
+      </c>
+      <c r="AE9" t="n">
+        <v>97</v>
+      </c>
+      <c r="AF9" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -1862,6 +1949,15 @@
         </is>
       </c>
       <c r="AC10" t="inlineStr"/>
+      <c r="AD10" t="n">
+        <v>65</v>
+      </c>
+      <c r="AE10" t="n">
+        <v>97</v>
+      </c>
+      <c r="AF10" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -2005,6 +2101,15 @@
         </is>
       </c>
       <c r="AC11" t="inlineStr"/>
+      <c r="AD11" t="n">
+        <v>65</v>
+      </c>
+      <c r="AE11" t="n">
+        <v>97</v>
+      </c>
+      <c r="AF11" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -2148,6 +2253,15 @@
         </is>
       </c>
       <c r="AC12" t="inlineStr"/>
+      <c r="AD12" t="n">
+        <v>65</v>
+      </c>
+      <c r="AE12" t="n">
+        <v>97</v>
+      </c>
+      <c r="AF12" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -2287,6 +2401,15 @@
       </c>
       <c r="AB13" t="inlineStr"/>
       <c r="AC13" t="inlineStr"/>
+      <c r="AD13" t="n">
+        <v>65</v>
+      </c>
+      <c r="AE13" t="n">
+        <v>97</v>
+      </c>
+      <c r="AF13" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -2430,6 +2553,15 @@
         </is>
       </c>
       <c r="AC14" t="inlineStr"/>
+      <c r="AD14" t="n">
+        <v>65</v>
+      </c>
+      <c r="AE14" t="n">
+        <v>97</v>
+      </c>
+      <c r="AF14" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -2573,6 +2705,15 @@
         </is>
       </c>
       <c r="AC15" t="inlineStr"/>
+      <c r="AD15" t="n">
+        <v>65</v>
+      </c>
+      <c r="AE15" t="n">
+        <v>97</v>
+      </c>
+      <c r="AF15" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -2716,6 +2857,15 @@
         </is>
       </c>
       <c r="AC16" t="inlineStr"/>
+      <c r="AD16" t="n">
+        <v>65</v>
+      </c>
+      <c r="AE16" t="n">
+        <v>97</v>
+      </c>
+      <c r="AF16" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -2855,6 +3005,15 @@
       </c>
       <c r="AB17" t="inlineStr"/>
       <c r="AC17" t="inlineStr"/>
+      <c r="AD17" t="n">
+        <v>65</v>
+      </c>
+      <c r="AE17" t="n">
+        <v>97</v>
+      </c>
+      <c r="AF17" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -2998,6 +3157,15 @@
         </is>
       </c>
       <c r="AC18" t="inlineStr"/>
+      <c r="AD18" t="n">
+        <v>65</v>
+      </c>
+      <c r="AE18" t="n">
+        <v>97</v>
+      </c>
+      <c r="AF18" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -3141,6 +3309,15 @@
         </is>
       </c>
       <c r="AC19" t="inlineStr"/>
+      <c r="AD19" t="n">
+        <v>65</v>
+      </c>
+      <c r="AE19" t="n">
+        <v>97</v>
+      </c>
+      <c r="AF19" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -3284,6 +3461,15 @@
         </is>
       </c>
       <c r="AC20" t="inlineStr"/>
+      <c r="AD20" t="n">
+        <v>65</v>
+      </c>
+      <c r="AE20" t="n">
+        <v>97</v>
+      </c>
+      <c r="AF20" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -3427,6 +3613,15 @@
         </is>
       </c>
       <c r="AC21" t="inlineStr"/>
+      <c r="AD21" t="n">
+        <v>65</v>
+      </c>
+      <c r="AE21" t="n">
+        <v>97</v>
+      </c>
+      <c r="AF21" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -3570,6 +3765,15 @@
         </is>
       </c>
       <c r="AC22" t="inlineStr"/>
+      <c r="AD22" t="n">
+        <v>65</v>
+      </c>
+      <c r="AE22" t="n">
+        <v>97</v>
+      </c>
+      <c r="AF22" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -3709,6 +3913,15 @@
       </c>
       <c r="AB23" t="inlineStr"/>
       <c r="AC23" t="inlineStr"/>
+      <c r="AD23" t="n">
+        <v>65</v>
+      </c>
+      <c r="AE23" t="n">
+        <v>97</v>
+      </c>
+      <c r="AF23" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -3852,6 +4065,15 @@
         </is>
       </c>
       <c r="AC24" t="inlineStr"/>
+      <c r="AD24" t="n">
+        <v>65</v>
+      </c>
+      <c r="AE24" t="n">
+        <v>97</v>
+      </c>
+      <c r="AF24" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -3991,6 +4213,15 @@
       </c>
       <c r="AB25" t="inlineStr"/>
       <c r="AC25" t="inlineStr"/>
+      <c r="AD25" t="n">
+        <v>65</v>
+      </c>
+      <c r="AE25" t="n">
+        <v>97</v>
+      </c>
+      <c r="AF25" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -4134,6 +4365,15 @@
         </is>
       </c>
       <c r="AC26" t="inlineStr"/>
+      <c r="AD26" t="n">
+        <v>65</v>
+      </c>
+      <c r="AE26" t="n">
+        <v>97</v>
+      </c>
+      <c r="AF26" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -4277,6 +4517,15 @@
         </is>
       </c>
       <c r="AC27" t="inlineStr"/>
+      <c r="AD27" t="n">
+        <v>65</v>
+      </c>
+      <c r="AE27" t="n">
+        <v>97</v>
+      </c>
+      <c r="AF27" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -4416,6 +4665,15 @@
       </c>
       <c r="AB28" t="inlineStr"/>
       <c r="AC28" t="inlineStr"/>
+      <c r="AD28" t="n">
+        <v>65</v>
+      </c>
+      <c r="AE28" t="n">
+        <v>97</v>
+      </c>
+      <c r="AF28" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -4559,6 +4817,15 @@
         </is>
       </c>
       <c r="AC29" t="inlineStr"/>
+      <c r="AD29" t="n">
+        <v>65</v>
+      </c>
+      <c r="AE29" t="n">
+        <v>97</v>
+      </c>
+      <c r="AF29" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -4702,6 +4969,15 @@
         </is>
       </c>
       <c r="AC30" t="inlineStr"/>
+      <c r="AD30" t="n">
+        <v>65</v>
+      </c>
+      <c r="AE30" t="n">
+        <v>97</v>
+      </c>
+      <c r="AF30" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -4841,6 +5117,15 @@
       </c>
       <c r="AB31" t="inlineStr"/>
       <c r="AC31" t="inlineStr"/>
+      <c r="AD31" t="n">
+        <v>65</v>
+      </c>
+      <c r="AE31" t="n">
+        <v>97</v>
+      </c>
+      <c r="AF31" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -4984,6 +5269,15 @@
         </is>
       </c>
       <c r="AC32" t="inlineStr"/>
+      <c r="AD32" t="n">
+        <v>65</v>
+      </c>
+      <c r="AE32" t="n">
+        <v>97</v>
+      </c>
+      <c r="AF32" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -5123,6 +5417,15 @@
       </c>
       <c r="AB33" t="inlineStr"/>
       <c r="AC33" t="inlineStr"/>
+      <c r="AD33" t="n">
+        <v>65</v>
+      </c>
+      <c r="AE33" t="n">
+        <v>97</v>
+      </c>
+      <c r="AF33" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -5262,6 +5565,15 @@
       </c>
       <c r="AB34" t="inlineStr"/>
       <c r="AC34" t="inlineStr"/>
+      <c r="AD34" t="n">
+        <v>65</v>
+      </c>
+      <c r="AE34" t="n">
+        <v>97</v>
+      </c>
+      <c r="AF34" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -5405,6 +5717,15 @@
         </is>
       </c>
       <c r="AC35" t="inlineStr"/>
+      <c r="AD35" t="n">
+        <v>65</v>
+      </c>
+      <c r="AE35" t="n">
+        <v>97</v>
+      </c>
+      <c r="AF35" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -5548,6 +5869,15 @@
         </is>
       </c>
       <c r="AC36" t="inlineStr"/>
+      <c r="AD36" t="n">
+        <v>65</v>
+      </c>
+      <c r="AE36" t="n">
+        <v>97</v>
+      </c>
+      <c r="AF36" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -5691,6 +6021,15 @@
         </is>
       </c>
       <c r="AC37" t="inlineStr"/>
+      <c r="AD37" t="n">
+        <v>65</v>
+      </c>
+      <c r="AE37" t="n">
+        <v>97</v>
+      </c>
+      <c r="AF37" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -5834,6 +6173,15 @@
         </is>
       </c>
       <c r="AC38" t="inlineStr"/>
+      <c r="AD38" t="n">
+        <v>65</v>
+      </c>
+      <c r="AE38" t="n">
+        <v>97</v>
+      </c>
+      <c r="AF38" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -5977,6 +6325,15 @@
         </is>
       </c>
       <c r="AC39" t="inlineStr"/>
+      <c r="AD39" t="n">
+        <v>65</v>
+      </c>
+      <c r="AE39" t="n">
+        <v>97</v>
+      </c>
+      <c r="AF39" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -6120,6 +6477,15 @@
         </is>
       </c>
       <c r="AC40" t="inlineStr"/>
+      <c r="AD40" t="n">
+        <v>65</v>
+      </c>
+      <c r="AE40" t="n">
+        <v>97</v>
+      </c>
+      <c r="AF40" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -6263,6 +6629,15 @@
         </is>
       </c>
       <c r="AC41" t="inlineStr"/>
+      <c r="AD41" t="n">
+        <v>65</v>
+      </c>
+      <c r="AE41" t="n">
+        <v>97</v>
+      </c>
+      <c r="AF41" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -6406,6 +6781,15 @@
         </is>
       </c>
       <c r="AC42" t="inlineStr"/>
+      <c r="AD42" t="n">
+        <v>65</v>
+      </c>
+      <c r="AE42" t="n">
+        <v>97</v>
+      </c>
+      <c r="AF42" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
@@ -6545,6 +6929,15 @@
       </c>
       <c r="AB43" t="inlineStr"/>
       <c r="AC43" t="inlineStr"/>
+      <c r="AD43" t="n">
+        <v>65</v>
+      </c>
+      <c r="AE43" t="n">
+        <v>97</v>
+      </c>
+      <c r="AF43" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
@@ -6684,6 +7077,15 @@
       </c>
       <c r="AB44" t="inlineStr"/>
       <c r="AC44" t="inlineStr"/>
+      <c r="AD44" t="n">
+        <v>65</v>
+      </c>
+      <c r="AE44" t="n">
+        <v>97</v>
+      </c>
+      <c r="AF44" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
@@ -6831,6 +7233,15 @@
           <t>All-Star</t>
         </is>
       </c>
+      <c r="AD45" t="n">
+        <v>65</v>
+      </c>
+      <c r="AE45" t="n">
+        <v>97</v>
+      </c>
+      <c r="AF45" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
@@ -6974,6 +7385,15 @@
         </is>
       </c>
       <c r="AC46" t="inlineStr"/>
+      <c r="AD46" t="n">
+        <v>65</v>
+      </c>
+      <c r="AE46" t="n">
+        <v>97</v>
+      </c>
+      <c r="AF46" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
@@ -7113,6 +7533,15 @@
       </c>
       <c r="AB47" t="inlineStr"/>
       <c r="AC47" t="inlineStr"/>
+      <c r="AD47" t="n">
+        <v>65</v>
+      </c>
+      <c r="AE47" t="n">
+        <v>97</v>
+      </c>
+      <c r="AF47" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
@@ -7252,6 +7681,15 @@
         </is>
       </c>
       <c r="AC48" t="inlineStr"/>
+      <c r="AD48" t="n">
+        <v>65</v>
+      </c>
+      <c r="AE48" t="n">
+        <v>97</v>
+      </c>
+      <c r="AF48" t="n">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>